<commit_message>
Update Flask app with Nominatim
</commit_message>
<xml_diff>
--- a/locations.xlsx
+++ b/locations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,24 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Karmayogi Bhavan, Road 3, Sector 7, Gandhinagar, Gandhinagar Taluka, Gandhinagar, Gujarat, 382008, India</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Karmayogi Bhavan, Road 3, Sector 7, Gandhinagar, Gandhinagar Taluka, Gandhinagar, Gujarat, 382008, India</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>